<commit_message>
Plan de test 70%
</commit_message>
<xml_diff>
--- a/PlanDeTests.xlsx
+++ b/PlanDeTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comto\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\home\etienne\Docs\INF3190\INF3190 TS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B47785E-1D6F-4F28-A5CB-9CFE12EC7C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6CBDC0-9297-4D2D-B94F-65BBC4378B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14520" yWindow="720" windowWidth="28560" windowHeight="30990" xr2:uid="{669C2AC5-E1DC-4B64-A776-4DF8109FDB75}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="148">
   <si>
     <t>Description des fonctionnalités</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Ajout d'un enfant</t>
   </si>
   <si>
-    <t>Suppression d'un enfant</t>
-  </si>
-  <si>
     <t>Modification d'un enfant</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>EF - 014</t>
-  </si>
-  <si>
     <t>ID des suites de tests</t>
   </si>
   <si>
@@ -171,9 +165,6 @@
     <t>ST - 013</t>
   </si>
   <si>
-    <t>ST - 014</t>
-  </si>
-  <si>
     <t>Ajout d'un programme au panier</t>
   </si>
   <si>
@@ -337,6 +328,156 @@
   </si>
   <si>
     <t>Création d'une Activité / Bloc activité et de type d'activité</t>
+  </si>
+  <si>
+    <t>CT - 020</t>
+  </si>
+  <si>
+    <t>CT - 021</t>
+  </si>
+  <si>
+    <t>CT - 022</t>
+  </si>
+  <si>
+    <t>CT - 023</t>
+  </si>
+  <si>
+    <t>CT - 024</t>
+  </si>
+  <si>
+    <t>Création d'un Type d'Activité</t>
+  </si>
+  <si>
+    <t>CT - 025</t>
+  </si>
+  <si>
+    <t>CT - 026</t>
+  </si>
+  <si>
+    <t>Sélection d'un Type d'Activité</t>
+  </si>
+  <si>
+    <t>Affichage des Types d'activités dans la liste déroulante</t>
+  </si>
+  <si>
+    <t>Faible</t>
+  </si>
+  <si>
+    <t>CT - 027</t>
+  </si>
+  <si>
+    <t>CT - 028</t>
+  </si>
+  <si>
+    <t>CT - 029</t>
+  </si>
+  <si>
+    <t>Couriel invalide</t>
+  </si>
+  <si>
+    <t>Avertissement que la forme est invalide</t>
+  </si>
+  <si>
+    <t>Date de naissance invalides</t>
+  </si>
+  <si>
+    <t>Avertisement que la date est impossible</t>
+  </si>
+  <si>
+    <t>Nom utilisateur déjà utilisé</t>
+  </si>
+  <si>
+    <t>Création d'un compte</t>
+  </si>
+  <si>
+    <t>Avertissement que le nom d'utilisateur est déjà pris</t>
+  </si>
+  <si>
+    <t>TP3</t>
+  </si>
+  <si>
+    <t>Prénom d'un caractère</t>
+  </si>
+  <si>
+    <t>Nom d'un caractère</t>
+  </si>
+  <si>
+    <t>Avertissement sur la longueur du nom</t>
+  </si>
+  <si>
+    <t>CT - 030</t>
+  </si>
+  <si>
+    <t>CT - 031</t>
+  </si>
+  <si>
+    <t>CT - 032</t>
+  </si>
+  <si>
+    <t>CT - 033</t>
+  </si>
+  <si>
+    <t>CT - 034</t>
+  </si>
+  <si>
+    <t>Message de succès et enregistrement dans la base de donnée</t>
+  </si>
+  <si>
+    <t>CT - 035</t>
+  </si>
+  <si>
+    <t>CT - 036</t>
+  </si>
+  <si>
+    <t>CT - 037</t>
+  </si>
+  <si>
+    <t>CT - 038</t>
+  </si>
+  <si>
+    <t>CT - 039</t>
+  </si>
+  <si>
+    <t>CT - 040</t>
+  </si>
+  <si>
+    <t>CT - 041</t>
+  </si>
+  <si>
+    <t>CT - 042</t>
+  </si>
+  <si>
+    <t>CT - 043</t>
+  </si>
+  <si>
+    <t>Même nom et prénom qu'un enfant existant</t>
+  </si>
+  <si>
+    <t>Création d'un enfant</t>
+  </si>
+  <si>
+    <t>Avertissement que cet enfant existe déjà</t>
+  </si>
+  <si>
+    <t>CT - 044</t>
+  </si>
+  <si>
+    <t>CT - 045</t>
+  </si>
+  <si>
+    <t>CT - 046</t>
+  </si>
+  <si>
+    <t>Ajout d'une note</t>
+  </si>
+  <si>
+    <t>Création d'un autre enfant</t>
+  </si>
+  <si>
+    <t>CT - 047</t>
+  </si>
+  <si>
+    <t>Supprimer un enfant</t>
   </si>
 </sst>
 </file>
@@ -704,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B873A8A6-6060-4A82-9BE9-F2B161063782}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E44" sqref="A38:E44"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,8 +856,8 @@
     <col min="1" max="1" width="34.140625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="68.5703125" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -724,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -738,7 +879,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -752,7 +893,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -766,7 +907,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -780,7 +921,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -794,7 +935,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -808,7 +949,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -822,7 +963,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -836,10 +977,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -850,10 +991,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
@@ -864,10 +1005,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -878,10 +1019,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>
@@ -892,10 +1033,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
@@ -906,133 +1047,133 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D15" t="s">
-        <v>29</v>
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>54</v>
+      <c r="B21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1040,155 +1181,155 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1199,139 +1340,765 @@
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="B50" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B51" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>54</v>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cas de test 100%
</commit_message>
<xml_diff>
--- a/PlanDeTests.xlsx
+++ b/PlanDeTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comto\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\home\etienne\Docs\INF3190\INF3190 TS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6CBDC0-9297-4D2D-B94F-65BBC4378B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2419180C-4679-4C37-A91C-95D9BA210375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14520" yWindow="720" windowWidth="28560" windowHeight="30990" xr2:uid="{669C2AC5-E1DC-4B64-A776-4DF8109FDB75}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="184">
   <si>
     <t>Description des fonctionnalités</t>
   </si>
@@ -42,27 +42,6 @@
     <t>ID des fonctionnalités</t>
   </si>
   <si>
-    <t>EF - 001</t>
-  </si>
-  <si>
-    <t>EF - 002</t>
-  </si>
-  <si>
-    <t>EF - 003</t>
-  </si>
-  <si>
-    <t>EF - 004</t>
-  </si>
-  <si>
-    <t>EF - 005</t>
-  </si>
-  <si>
-    <t>EF - 006</t>
-  </si>
-  <si>
-    <t>EF - 007</t>
-  </si>
-  <si>
     <t>Insertion d'une Session</t>
   </si>
   <si>
@@ -84,24 +63,6 @@
     <t>Insertion d'une Activité</t>
   </si>
   <si>
-    <t>EF - 008</t>
-  </si>
-  <si>
-    <t>EF - 009</t>
-  </si>
-  <si>
-    <t>EF - 010</t>
-  </si>
-  <si>
-    <t>EF - 011</t>
-  </si>
-  <si>
-    <t>EF - 012</t>
-  </si>
-  <si>
-    <t>EF - 013</t>
-  </si>
-  <si>
     <t>/accueil/inscription</t>
   </si>
   <si>
@@ -126,45 +87,6 @@
     <t>ID des suites de tests</t>
   </si>
   <si>
-    <t>ST - 001</t>
-  </si>
-  <si>
-    <t>ST - 002</t>
-  </si>
-  <si>
-    <t>ST - 003</t>
-  </si>
-  <si>
-    <t>ST - 004</t>
-  </si>
-  <si>
-    <t>ST - 005</t>
-  </si>
-  <si>
-    <t>ST - 006</t>
-  </si>
-  <si>
-    <t>ST - 007</t>
-  </si>
-  <si>
-    <t>ST - 008</t>
-  </si>
-  <si>
-    <t>ST - 009</t>
-  </si>
-  <si>
-    <t>ST - 010</t>
-  </si>
-  <si>
-    <t>ST - 011</t>
-  </si>
-  <si>
-    <t>ST - 012</t>
-  </si>
-  <si>
-    <t>ST - 013</t>
-  </si>
-  <si>
     <t>Ajout d'un programme au panier</t>
   </si>
   <si>
@@ -192,63 +114,6 @@
     <t>Priorité</t>
   </si>
   <si>
-    <t>CT - 001</t>
-  </si>
-  <si>
-    <t>CT - 002</t>
-  </si>
-  <si>
-    <t>CT - 003</t>
-  </si>
-  <si>
-    <t>CT - 004</t>
-  </si>
-  <si>
-    <t>CT - 005</t>
-  </si>
-  <si>
-    <t>CT - 006</t>
-  </si>
-  <si>
-    <t>CT - 007</t>
-  </si>
-  <si>
-    <t>CT - 008</t>
-  </si>
-  <si>
-    <t>CT - 009</t>
-  </si>
-  <si>
-    <t>CT - 010</t>
-  </si>
-  <si>
-    <t>CT - 011</t>
-  </si>
-  <si>
-    <t>CT - 012</t>
-  </si>
-  <si>
-    <t>CT - 013</t>
-  </si>
-  <si>
-    <t>CT - 014</t>
-  </si>
-  <si>
-    <t>CT - 015</t>
-  </si>
-  <si>
-    <t>CT - 016</t>
-  </si>
-  <si>
-    <t>CT - 017</t>
-  </si>
-  <si>
-    <t>CT - 018</t>
-  </si>
-  <si>
-    <t>CT - 019</t>
-  </si>
-  <si>
     <t>Champs vides</t>
   </si>
   <si>
@@ -330,30 +195,9 @@
     <t>Création d'une Activité / Bloc activité et de type d'activité</t>
   </si>
   <si>
-    <t>CT - 020</t>
-  </si>
-  <si>
-    <t>CT - 021</t>
-  </si>
-  <si>
-    <t>CT - 022</t>
-  </si>
-  <si>
-    <t>CT - 023</t>
-  </si>
-  <si>
-    <t>CT - 024</t>
-  </si>
-  <si>
     <t>Création d'un Type d'Activité</t>
   </si>
   <si>
-    <t>CT - 025</t>
-  </si>
-  <si>
-    <t>CT - 026</t>
-  </si>
-  <si>
     <t>Sélection d'un Type d'Activité</t>
   </si>
   <si>
@@ -363,15 +207,6 @@
     <t>Faible</t>
   </si>
   <si>
-    <t>CT - 027</t>
-  </si>
-  <si>
-    <t>CT - 028</t>
-  </si>
-  <si>
-    <t>CT - 029</t>
-  </si>
-  <si>
     <t>Couriel invalide</t>
   </si>
   <si>
@@ -405,51 +240,9 @@
     <t>Avertissement sur la longueur du nom</t>
   </si>
   <si>
-    <t>CT - 030</t>
-  </si>
-  <si>
-    <t>CT - 031</t>
-  </si>
-  <si>
-    <t>CT - 032</t>
-  </si>
-  <si>
-    <t>CT - 033</t>
-  </si>
-  <si>
-    <t>CT - 034</t>
-  </si>
-  <si>
     <t>Message de succès et enregistrement dans la base de donnée</t>
   </si>
   <si>
-    <t>CT - 035</t>
-  </si>
-  <si>
-    <t>CT - 036</t>
-  </si>
-  <si>
-    <t>CT - 037</t>
-  </si>
-  <si>
-    <t>CT - 038</t>
-  </si>
-  <si>
-    <t>CT - 039</t>
-  </si>
-  <si>
-    <t>CT - 040</t>
-  </si>
-  <si>
-    <t>CT - 041</t>
-  </si>
-  <si>
-    <t>CT - 042</t>
-  </si>
-  <si>
-    <t>CT - 043</t>
-  </si>
-  <si>
     <t>Même nom et prénom qu'un enfant existant</t>
   </si>
   <si>
@@ -459,25 +252,340 @@
     <t>Avertissement que cet enfant existe déjà</t>
   </si>
   <si>
-    <t>CT - 044</t>
-  </si>
-  <si>
-    <t>CT - 045</t>
-  </si>
-  <si>
-    <t>CT - 046</t>
-  </si>
-  <si>
     <t>Ajout d'une note</t>
   </si>
   <si>
     <t>Création d'un autre enfant</t>
   </si>
   <si>
-    <t>CT - 047</t>
-  </si>
-  <si>
     <t>Supprimer un enfant</t>
+  </si>
+  <si>
+    <t>Création d'un parent</t>
+  </si>
+  <si>
+    <t>Modification du nom et prénom</t>
+  </si>
+  <si>
+    <t>Modification de l'adresse</t>
+  </si>
+  <si>
+    <t>Création d'un parent et d'enfants</t>
+  </si>
+  <si>
+    <t>Sauvegarde dans la base de donnée et affichage des adresses aux enfants</t>
+  </si>
+  <si>
+    <t>EF.001</t>
+  </si>
+  <si>
+    <t>EF.002</t>
+  </si>
+  <si>
+    <t>EF.003</t>
+  </si>
+  <si>
+    <t>EF.004</t>
+  </si>
+  <si>
+    <t>EF.005</t>
+  </si>
+  <si>
+    <t>EF.006</t>
+  </si>
+  <si>
+    <t>EF.007</t>
+  </si>
+  <si>
+    <t>EF.008</t>
+  </si>
+  <si>
+    <t>EF.009</t>
+  </si>
+  <si>
+    <t>EF.010</t>
+  </si>
+  <si>
+    <t>EF.011</t>
+  </si>
+  <si>
+    <t>EF.012</t>
+  </si>
+  <si>
+    <t>EF.013</t>
+  </si>
+  <si>
+    <t>ST.001</t>
+  </si>
+  <si>
+    <t>ST.002</t>
+  </si>
+  <si>
+    <t>ST.003</t>
+  </si>
+  <si>
+    <t>ST.004</t>
+  </si>
+  <si>
+    <t>ST.005</t>
+  </si>
+  <si>
+    <t>ST.006</t>
+  </si>
+  <si>
+    <t>ST.007</t>
+  </si>
+  <si>
+    <t>ST.008</t>
+  </si>
+  <si>
+    <t>ST.009</t>
+  </si>
+  <si>
+    <t>ST.010</t>
+  </si>
+  <si>
+    <t>ST.011</t>
+  </si>
+  <si>
+    <t>ST.012</t>
+  </si>
+  <si>
+    <t>ST.013</t>
+  </si>
+  <si>
+    <t>CT.001</t>
+  </si>
+  <si>
+    <t>CT.002</t>
+  </si>
+  <si>
+    <t>CT.003</t>
+  </si>
+  <si>
+    <t>CT.004</t>
+  </si>
+  <si>
+    <t>CT.005</t>
+  </si>
+  <si>
+    <t>CT.006</t>
+  </si>
+  <si>
+    <t>CT.007</t>
+  </si>
+  <si>
+    <t>CT.008</t>
+  </si>
+  <si>
+    <t>CT.009</t>
+  </si>
+  <si>
+    <t>CT.010</t>
+  </si>
+  <si>
+    <t>CT.011</t>
+  </si>
+  <si>
+    <t>CT.012</t>
+  </si>
+  <si>
+    <t>CT.013</t>
+  </si>
+  <si>
+    <t>CT.014</t>
+  </si>
+  <si>
+    <t>CT.015</t>
+  </si>
+  <si>
+    <t>CT.016</t>
+  </si>
+  <si>
+    <t>CT.017</t>
+  </si>
+  <si>
+    <t>CT.018</t>
+  </si>
+  <si>
+    <t>CT.019</t>
+  </si>
+  <si>
+    <t>CT.020</t>
+  </si>
+  <si>
+    <t>CT.021</t>
+  </si>
+  <si>
+    <t>CT.022</t>
+  </si>
+  <si>
+    <t>CT.023</t>
+  </si>
+  <si>
+    <t>CT.024</t>
+  </si>
+  <si>
+    <t>CT.025</t>
+  </si>
+  <si>
+    <t>CT.026</t>
+  </si>
+  <si>
+    <t>CT.027</t>
+  </si>
+  <si>
+    <t>CT.028</t>
+  </si>
+  <si>
+    <t>CT.029</t>
+  </si>
+  <si>
+    <t>CT.030</t>
+  </si>
+  <si>
+    <t>CT.031</t>
+  </si>
+  <si>
+    <t>CT.032</t>
+  </si>
+  <si>
+    <t>CT.033</t>
+  </si>
+  <si>
+    <t>CT.034</t>
+  </si>
+  <si>
+    <t>CT.035</t>
+  </si>
+  <si>
+    <t>CT.036</t>
+  </si>
+  <si>
+    <t>CT.037</t>
+  </si>
+  <si>
+    <t>CT.038</t>
+  </si>
+  <si>
+    <t>CT.039</t>
+  </si>
+  <si>
+    <t>CT.040</t>
+  </si>
+  <si>
+    <t>CT.041</t>
+  </si>
+  <si>
+    <t>CT.042</t>
+  </si>
+  <si>
+    <t>CT.043</t>
+  </si>
+  <si>
+    <t>CT.044</t>
+  </si>
+  <si>
+    <t>CT.045</t>
+  </si>
+  <si>
+    <t>CT.046</t>
+  </si>
+  <si>
+    <t>CT.047</t>
+  </si>
+  <si>
+    <t>CT.048</t>
+  </si>
+  <si>
+    <t>CT.049</t>
+  </si>
+  <si>
+    <t>CT.050</t>
+  </si>
+  <si>
+    <t>CT.051</t>
+  </si>
+  <si>
+    <t>CT.052</t>
+  </si>
+  <si>
+    <t>CT.053</t>
+  </si>
+  <si>
+    <t>CT.054</t>
+  </si>
+  <si>
+    <t>CT.055</t>
+  </si>
+  <si>
+    <t>CT.056</t>
+  </si>
+  <si>
+    <t>Ajout d'un programme échu</t>
+  </si>
+  <si>
+    <t>Ajout d'un programme payé</t>
+  </si>
+  <si>
+    <t>Imposible d'ajouter au panier</t>
+  </si>
+  <si>
+    <t>Compte parent et enfant. Semaine passé</t>
+  </si>
+  <si>
+    <t>Compte parent et enfant. Semaine payé</t>
+  </si>
+  <si>
+    <t>CT.057</t>
+  </si>
+  <si>
+    <t>Ajout d'un programme valide</t>
+  </si>
+  <si>
+    <t>Compte parent et enfant</t>
+  </si>
+  <si>
+    <t>Montant ajusté au panier, indiquation que programme au panier</t>
+  </si>
+  <si>
+    <t>Ajout de programmes valides</t>
+  </si>
+  <si>
+    <t>CT.058</t>
+  </si>
+  <si>
+    <t>CT.059</t>
+  </si>
+  <si>
+    <t>CT.060</t>
+  </si>
+  <si>
+    <t>Retrait d'un programme au panier</t>
+  </si>
+  <si>
+    <t>Montant ajusté au panier, indiquation qu'il est possible d'ajouter au panier</t>
+  </si>
+  <si>
+    <t>Selection d'un programme</t>
+  </si>
+  <si>
+    <t>Affichage des Programmes disponibles pour cette semaine dans la liste déroulante</t>
+  </si>
+  <si>
+    <t>CT.061</t>
+  </si>
+  <si>
+    <t>CT.062</t>
+  </si>
+  <si>
+    <t>Paiement du panier</t>
+  </si>
+  <si>
+    <t>Compte parent et enfant. Programme au panier.</t>
+  </si>
+  <si>
+    <t>Enregistrement des inscriptions dans la base de donnée et affichage des semaines payées</t>
   </si>
 </sst>
 </file>
@@ -845,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B873A8A6-6060-4A82-9BE9-F2B161063782}">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,306 +973,305 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1172,7 +1279,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1181,159 +1288,158 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1341,7 +1447,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1350,755 +1456,1059 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>116</v>
+        <v>61</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>138</v>
+        <v>69</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>138</v>
+        <v>69</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>144</v>
+        <v>72</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>147</v>
+        <v>74</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="E89" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>27</v>
+      <c r="C90" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>51</v>
+      <c r="A92" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B103" t="s">
+        <v>162</v>
+      </c>
+      <c r="C103" t="s">
+        <v>165</v>
+      </c>
+      <c r="D103" t="s">
+        <v>164</v>
+      </c>
+      <c r="E103" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B104" t="s">
+        <v>163</v>
+      </c>
+      <c r="C104" t="s">
+        <v>166</v>
+      </c>
+      <c r="D104" t="s">
+        <v>164</v>
+      </c>
+      <c r="E104" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B105" t="s">
+        <v>168</v>
+      </c>
+      <c r="C105" t="s">
+        <v>169</v>
+      </c>
+      <c r="D105" t="s">
+        <v>170</v>
+      </c>
+      <c r="E105" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B106" t="s">
+        <v>171</v>
+      </c>
+      <c r="C106" t="s">
+        <v>169</v>
+      </c>
+      <c r="D106" t="s">
+        <v>170</v>
+      </c>
+      <c r="E106" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B107" t="s">
+        <v>177</v>
+      </c>
+      <c r="C107" t="s">
+        <v>169</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E107" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B111" t="s">
+        <v>175</v>
+      </c>
+      <c r="C111" t="s">
+        <v>169</v>
+      </c>
+      <c r="D111" t="s">
+        <v>176</v>
+      </c>
+      <c r="E111" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B115" t="s">
+        <v>181</v>
+      </c>
+      <c r="C115" t="s">
+        <v>182</v>
+      </c>
+      <c r="D115" t="s">
+        <v>183</v>
+      </c>
+      <c r="E115" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>